<commit_message>
Actualizar formulario de autoevaluación
</commit_message>
<xml_diff>
--- a/evaluaciones/MiApellidoMiNombre-2018MMDD.xlsx
+++ b/evaluaciones/MiApellidoMiNombre-2018MMDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\teaching\grado\asignaturas\PWEB Proyectos para la web\2018-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kI+lo06StZM5GtepswRN6DAf4mK02ZCokfy3PuQxWcTh6w4FNxyVRMFhT1TaqWKlxwk8FCvlDCjZMhwgTvBCFA==" workbookSaltValue="ehpoaGy4ztBerVs6gjvzoQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="sfa08O3KF67PVIPzK4OFLnWpIviH6O1fzBYR8+obEZCg6Od3XF+NyjrukVRbun4esNZvvjBYVMNNt2kZq2K1mQ==" workbookSaltValue="vjVhSBHXzad4thLlwEQ/+g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Autoevaluación de reunión en equipo base</t>
   </si>
@@ -33,24 +33,12 @@
     <t>Yo</t>
   </si>
   <si>
-    <t>Indicador 1</t>
-  </si>
-  <si>
-    <t>Indicador 2</t>
-  </si>
-  <si>
     <t>Asistencia</t>
   </si>
   <si>
     <t>Participación</t>
   </si>
   <si>
-    <t>Indicador 3</t>
-  </si>
-  <si>
-    <t>Indicador 4</t>
-  </si>
-  <si>
     <t>Profesionalidad</t>
   </si>
   <si>
@@ -75,20 +63,201 @@
     <t xml:space="preserve">Rellena el cuadro azul con tu número de grupo, la fecha de la reunión a la que se refiere esta evaluación, tu nombre y los del resto de participantes en tu grupo. </t>
   </si>
   <si>
-    <t xml:space="preserve">Desupés introduce valores del 1 al 5 para cada indicador, tanto para tu autoevaluación como para el resto de participantes. </t>
-  </si>
-  <si>
     <t>Finalmente, renombra este archivo adecuadamente (añadiendo el número de grupo, tu nombre y la fecha de la reunión en el formato indicado) y añadelo  al branch "evaluaciones-tunombre" de tu fork personal del repositorio del equipo.</t>
   </si>
   <si>
     <t>Indicaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desupés introduce el valor correspondiente para cada indicador, tanto para tu autoevaluación como para el resto de participantes. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asiste a la reunión 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Está presente durante la mayor parte de la reunión 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3=100%, 2=más de 60%, 1=más de 40%, 0=menos de 40%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha justificado su ausencia 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí o N/A, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha avisado con al menos 24h de antelación 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí o N/A, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha entregado puntualmente las tareas que tenía asignadas 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha aportado ideas 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Permite la retroalimentación de ideas 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Es capaz de proponer un camino de acción 
+y se asegura de que ese camino tenga una meta/fin 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3=excelente, 2=bien, 1=regular, 0=nada</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha cumplido con los plazos asignados para la entrega de trabajos 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha mostrado implicación con el proyecto 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3=mucha, 2=bastante, 1=algo, 0=ninguna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha mostrado respeto con el resto de opiniones 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3=mucho, 2=bastante, 1=algo, 0=ninguno</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ha asumido con honestidad los errores que ha podido cometer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1=sí, 0=no</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +345,12 @@
       <i/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -357,16 +532,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -395,9 +567,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -423,32 +592,53 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,498 +924,498 @@
   <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.5703125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="49" style="18" customWidth="1"/>
-    <col min="4" max="7" width="4" style="18" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="18" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="18"/>
+    <col min="1" max="2" width="2.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" style="17" customWidth="1"/>
+    <col min="4" max="7" width="4" style="17" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="14"/>
-      <c r="J3" s="19" t="s">
-        <v>18</v>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="15"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-      <c r="C5" s="5">
+      <c r="B5" s="12"/>
+      <c r="C5" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="44"/>
+      <c r="D5" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="40"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="16"/>
-      <c r="J5" s="23" t="s">
-        <v>15</v>
+      <c r="H5" s="15"/>
+      <c r="J5" s="38" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
-      <c r="C6" s="6">
+      <c r="B6" s="12"/>
+      <c r="C6" s="5">
         <v>43353</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="45"/>
+      <c r="D6" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="41"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="17"/>
-      <c r="J6" s="23"/>
+      <c r="H6" s="16"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="45" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="45"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="16"/>
-      <c r="J7" s="23"/>
+      <c r="H7" s="15"/>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="46">
+      <c r="B8" s="12"/>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="36">
         <v>1</v>
       </c>
-      <c r="E8" s="47"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="16"/>
-      <c r="J8" s="23"/>
+      <c r="H8" s="15"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="46">
+      <c r="B9" s="12"/>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="36">
         <v>2</v>
       </c>
-      <c r="E9" s="47"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="16"/>
-      <c r="J9" s="23"/>
+      <c r="H9" s="15"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="46">
+      <c r="B10" s="12"/>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="36">
         <v>3</v>
       </c>
-      <c r="E10" s="47"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="16"/>
-      <c r="J10" s="23" t="s">
-        <v>16</v>
+      <c r="H10" s="15"/>
+      <c r="J10" s="38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="16"/>
-      <c r="J11" s="23"/>
+      <c r="H11" s="15"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="36"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="16"/>
-      <c r="J12" s="23"/>
+      <c r="H12" s="15"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="J13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="25"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="26" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="24">
         <v>1</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="24">
         <v>2</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="24">
         <v>3</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="J14" s="43"/>
-    </row>
-    <row r="15" spans="2:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="8" t="s">
+      <c r="H14" s="25"/>
+      <c r="J14" s="35"/>
+    </row>
+    <row r="15" spans="2:10" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <f>D16*0.39+D17/3*0.16+D18*0.29+D19*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" ref="E15:G15" si="0">E16*0.39+E17/3*0.16+E18*0.29+E19*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="J15" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="23"/>
+      <c r="C16" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="28"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B17" s="23"/>
+      <c r="C17" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="28"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="23"/>
+      <c r="C18" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="28"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="23"/>
+      <c r="C19" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="28"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="29"/>
+      <c r="C20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <f>D21*0.33+D22*0.24+D23*0.23+D24/3*0.19</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" ref="E20:G20" si="1">E21*0.33+E22*0.24+E23*0.23+E24/3*0.19</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="J20" s="38"/>
+    </row>
+    <row r="21" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B21" s="23"/>
+      <c r="C21" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="28"/>
+      <c r="J21" s="38"/>
+    </row>
+    <row r="22" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B22" s="23"/>
+      <c r="C22" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="28"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="23"/>
+      <c r="C23" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="28"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="2:10" ht="35.25" x14ac:dyDescent="0.2">
+      <c r="B24" s="23"/>
+      <c r="C24" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="28"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="2:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="29"/>
+      <c r="C25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="e">
-        <f>AVERAGE(D16:D19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E15" s="9" t="e">
-        <f t="shared" ref="E15:G15" si="0">AVERAGE(E16:E19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="J15" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="25"/>
-      <c r="C16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="30"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
-      <c r="C17" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="30"/>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="25"/>
-      <c r="C18" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="30"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="30"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="2:10" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
-      <c r="C20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9" t="e">
-        <f>AVERAGE(D21:D24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="9" t="e">
-        <f t="shared" ref="E20:G20" si="1">AVERAGE(E21:E24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="9" t="e">
-        <f>AVERAGE(G22:G24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="29"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="25"/>
-      <c r="C21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="30"/>
-      <c r="J21" s="23"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
-      <c r="C22" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="30"/>
-      <c r="J22" s="43"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="25"/>
-      <c r="C23" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="30"/>
-      <c r="J23" s="43"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="25"/>
-      <c r="C24" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="30"/>
-      <c r="J24" s="43"/>
-    </row>
-    <row r="25" spans="2:10" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
-      <c r="C25" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="9" t="e">
-        <f>AVERAGE(D26:D29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="9" t="e">
-        <f t="shared" ref="E25:G25" si="2">AVERAGE(E26:E29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="9" t="e">
+      <c r="D25" s="8">
+        <f>D26*0.38+D27/3*0.32+D28/3*0.17+D29*0.13</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" ref="E25:G25" si="2">E26*0.38+E27/3*0.32+E28/3*0.17+E29*0.13</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="29"/>
-      <c r="J25" s="43"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="25"/>
-      <c r="C26" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="30"/>
-      <c r="J26" s="43"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
-      <c r="C27" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="30"/>
-      <c r="J27" s="43"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="25"/>
-      <c r="C28" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="30"/>
-      <c r="J28" s="43"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="25"/>
-      <c r="C29" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="30"/>
-      <c r="J29" s="43"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="27"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B26" s="23"/>
+      <c r="C26" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="28"/>
+      <c r="J26" s="35"/>
+    </row>
+    <row r="27" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B27" s="23"/>
+      <c r="C27" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="28"/>
+      <c r="J27" s="35"/>
+    </row>
+    <row r="28" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B28" s="23"/>
+      <c r="C28" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="28"/>
+      <c r="J28" s="35"/>
+    </row>
+    <row r="29" spans="2:10" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B29" s="23"/>
+      <c r="C29" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="28"/>
+      <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="32"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="2:10" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="q3gdbVNKHe1CdZsn+Wt26/NT2y0jo1NjV5SNSkx8TqXMR5UmGRscG4grfqdnrdptf3ot1YV1W6y0AJwNhBFaiQ==" saltValue="MJNie36WU5p9wIuI6mz94A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="J5:J9"/>
     <mergeCell ref="J10:J13"/>
@@ -1235,10 +1425,18 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:H19 D26:H29 D21:F24 H21:H24 G22:G24">
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H21:H24 H16:H19 H26:H29">
       <formula1>1</formula1>
       <formula2>5</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:G16 D18:G19 D21:G23 D26:G26 D29:G29">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:G17 D24:G24 D27:G28">
+      <formula1>0</formula1>
+      <formula2>3</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>